<commit_message>
week 3 inning update
</commit_message>
<xml_diff>
--- a/data/schedules/Spring2023Schedule.xlsx
+++ b/data/schedules/Spring2023Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berry\GolandProjects\magic-8ball\data\schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9F199A-BCB4-4753-8D9C-790E2160567E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1429379A-04E0-491B-9039-24B1DF2F6900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18435" yWindow="2025" windowWidth="16410" windowHeight="11295" xr2:uid="{9584355D-9510-432C-A84B-A2CEEF79C7DD}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="37">
   <si>
     <t>Record</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>Shelia Lowe</t>
   </si>
 </sst>
 </file>
@@ -542,7 +545,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -552,9 +555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA30A97-9145-4EDA-8DB9-44B6A1233BAB}">
   <dimension ref="A2:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C24" sqref="C24"/>
+      <selection pane="topRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,10 +674,10 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
@@ -717,22 +720,22 @@
       </c>
       <c r="R3" s="6">
         <f>COUNTIF(B3:Q3, "W")/(COUNTIF(B3:Q3, "W")+COUNTIF(B3:Q3, "L"))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S3">
         <v>6</v>
       </c>
       <c r="T3">
         <f>MAX(S3-COUNTIF(B3:Q3, "W")-COUNTIF(B3:Q3, "L"), 0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U3">
         <f t="shared" ref="U3:U10" si="1">COUNTIF(B3:Q3, "A")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V10" si="2">U3-T3</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W3" t="s">
         <v>23</v>
@@ -746,10 +749,10 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
         <v>29</v>
@@ -790,20 +793,20 @@
       <c r="Q4" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="6" t="e">
+      <c r="R4" s="6">
         <f t="shared" ref="R4:R10" si="3">COUNTIF(B4:Q4, "W")/(COUNTIF(B4:Q4, "W")+COUNTIF(B4:Q4, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="S4">
         <v>6</v>
       </c>
       <c r="T4">
         <f t="shared" ref="T4:T10" si="4">MAX(S4-COUNTIF(B4:Q4, "W")-COUNTIF(B4:Q4, "L"), 0)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U4">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V4">
         <f t="shared" si="2"/>
@@ -821,10 +824,10 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
@@ -865,24 +868,24 @@
       <c r="Q5" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="6" t="e">
+      <c r="R5" s="6">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <v>6</v>
       </c>
       <c r="T5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U5">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V5">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W5" t="s">
         <v>7</v>
@@ -896,10 +899,10 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
@@ -940,24 +943,24 @@
       <c r="Q6" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="6" t="e">
+      <c r="R6" s="6">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <v>6</v>
       </c>
       <c r="T6">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U6">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V6">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W6" t="s">
         <v>13</v>
@@ -971,7 +974,7 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
@@ -1017,18 +1020,18 @@
       </c>
       <c r="R7" s="6">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S7">
         <v>6</v>
       </c>
       <c r="T7">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U7">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V7">
         <f t="shared" si="2"/>
@@ -1046,10 +1049,10 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -1090,24 +1093,24 @@
       <c r="Q8" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="6" t="e">
+      <c r="R8" s="6">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <v>6</v>
       </c>
       <c r="T8">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U8">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V8">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W8" t="s">
         <v>11</v>
@@ -1121,10 +1124,10 @@
         <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -1165,20 +1168,20 @@
       <c r="Q9" t="s">
         <v>29</v>
       </c>
-      <c r="R9" s="6" t="e">
+      <c r="R9" s="6">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S9">
         <v>6</v>
       </c>
       <c r="T9">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U9">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V9">
         <f t="shared" si="2"/>
@@ -1196,10 +1199,10 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -1242,22 +1245,22 @@
       </c>
       <c r="R10" s="6">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S10">
         <v>6</v>
       </c>
       <c r="T10">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U10">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V10">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W10" t="s">
         <v>18</v>
@@ -1271,13 +1274,13 @@
         <f t="shared" ref="B11:Q11" si="5">COUNTIF(B3:B10, "W")/(COUNTIF(B3:B10, "W")+COUNTIF(B3:B10, "L"))</f>
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="e">
+      <c r="C11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="5" t="e">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>0.2</v>
       </c>
       <c r="E11" s="5" t="e">
         <f t="shared" si="5"/>
@@ -1333,7 +1336,7 @@
       </c>
       <c r="R11" s="7">
         <f>AVERAGEIF(B11:Q11, "&gt;=0")</f>
-        <v>1</v>
+        <v>0.46666666666666662</v>
       </c>
       <c r="S11" s="2">
         <f>SUM(S3:S10)</f>
@@ -1341,15 +1344,15 @@
       </c>
       <c r="T11" s="2">
         <f>SUM(T3:T10)</f>
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="U11" s="2">
         <f>SUM(U3:U10)</f>
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="V11" s="2">
         <f>SUM(V3:V10)</f>
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -1446,10 +1449,10 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
@@ -1490,20 +1493,20 @@
       <c r="Q15" t="s">
         <v>29</v>
       </c>
-      <c r="R15" s="6" t="e">
+      <c r="R15" s="6">
         <f>COUNTIF(B15:Q15, "W")/(COUNTIF(B15:Q15, "W")+COUNTIF(B15:Q15, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0.5</v>
       </c>
       <c r="S15">
         <v>6</v>
       </c>
       <c r="T15">
         <f>MAX(S15-COUNTIF(B15:Q15, "W")-COUNTIF(B15:Q15, "L"), 0)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="U15">
         <f t="shared" ref="U15:U20" si="7">COUNTIF(B15:Q15, "A")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V15">
         <f t="shared" ref="V15:V20" si="8">U15-T15</f>
@@ -1521,10 +1524,10 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -1565,24 +1568,24 @@
       <c r="Q16" t="s">
         <v>29</v>
       </c>
-      <c r="R16" s="6" t="e">
+      <c r="R16" s="6">
         <f t="shared" ref="R16:R22" si="9">COUNTIF(B16:Q16, "W")/(COUNTIF(B16:Q16, "W")+COUNTIF(B16:Q16, "L"))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S16">
         <v>6</v>
       </c>
       <c r="T16">
         <f t="shared" ref="T16:T22" si="10">MAX(S16-COUNTIF(B16:Q16, "W")-COUNTIF(B16:Q16, "L"), 0)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U16">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V16">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W16" t="s">
         <v>11</v>
@@ -1590,16 +1593,16 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
         <v>29</v>
@@ -1642,7 +1645,7 @@
       </c>
       <c r="R17" s="6">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <v>6</v>
@@ -1653,11 +1656,11 @@
       </c>
       <c r="U17">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V17">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="W17" t="s">
         <v>23</v>
@@ -1671,7 +1674,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
         <v>30</v>
@@ -1717,18 +1720,18 @@
       </c>
       <c r="R18" s="6">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S18">
         <v>6</v>
       </c>
       <c r="T18">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U18">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V18">
         <f t="shared" si="8"/>
@@ -1746,10 +1749,10 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -1792,22 +1795,22 @@
       </c>
       <c r="R19" s="6">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="S19">
         <v>6</v>
       </c>
       <c r="T19">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U19">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V19">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="W19" t="s">
         <v>18</v>
@@ -1821,10 +1824,10 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
@@ -1878,11 +1881,11 @@
       </c>
       <c r="U20">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V20">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="W20" t="s">
         <v>28</v>
@@ -1896,10 +1899,10 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
         <v>29</v>
@@ -1940,24 +1943,24 @@
       <c r="Q21" t="s">
         <v>29</v>
       </c>
-      <c r="R21" s="6" t="e">
+      <c r="R21" s="6">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="S21">
         <v>6</v>
       </c>
       <c r="T21">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U21">
         <f>COUNTIF(B21:Q21, "A")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V21">
         <f>U21-T21</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="W21" t="s">
         <v>27</v>
@@ -1971,7 +1974,7 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
         <v>29</v>
@@ -2017,18 +2020,18 @@
       </c>
       <c r="R22" s="6">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S22">
         <v>6</v>
       </c>
       <c r="T22">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U22">
         <f>COUNTIF(B22:Q22, "A")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V22">
         <f>U22-T22</f>
@@ -2044,15 +2047,15 @@
       </c>
       <c r="B23" s="5">
         <f>COUNTIF(B15:B22, "W")/(COUNTIF(B15:B22, "W")+COUNTIF(B15:B22, "L"))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" ref="C23:D23" si="11">COUNTIF(C15:C22, "W")/(COUNTIF(C15:C22, "W")+COUNTIF(C15:C22, "L"))</f>
         <v>0.5</v>
       </c>
-      <c r="C23" s="5" t="e">
-        <f t="shared" ref="C23:D23" si="11">COUNTIF(C15:C22, "W")/(COUNTIF(C15:C22, "W")+COUNTIF(C15:C22, "L"))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D23" s="5" t="e">
+      <c r="D23" s="5">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>0.25</v>
       </c>
       <c r="E23" s="5" t="e">
         <f t="shared" ref="E23" si="12">COUNTIF(E15:E22, "W")/(COUNTIF(E15:E22, "W")+COUNTIF(E15:E22, "L"))</f>
@@ -2108,7 +2111,7 @@
       </c>
       <c r="R23" s="7">
         <f>AVERAGEIF(B23:Q23, "&gt;=0")</f>
-        <v>0.5</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="S23" s="2">
         <f>SUM(S15:S22)</f>
@@ -2116,15 +2119,15 @@
       </c>
       <c r="T23" s="2">
         <f>SUM(T15:T22)</f>
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="U23" s="2">
         <f>SUM(U15:U22)</f>
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="V23" s="2">
         <f>SUM(V15:V22)</f>
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>